<commit_message>
Updated to handle Flat Files
</commit_message>
<xml_diff>
--- a/ETL-DesignPatterns/Databases/Admin/Manual Scripts/Metadata.xlsx
+++ b/ETL-DesignPatterns/Databases/Admin/Manual Scripts/Metadata.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="13209" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23451" windowHeight="13209"/>
   </bookViews>
   <sheets>
     <sheet name="Connection" sheetId="2" r:id="rId1"/>
     <sheet name="Project" sheetId="1" r:id="rId2"/>
+    <sheet name="Item" sheetId="3" r:id="rId3"/>
+    <sheet name="ItemColumn" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="140">
   <si>
     <t>ProjectName</t>
   </si>
@@ -174,7 +176,277 @@
     <t>Data Source=.;Initial Catalog=Admin;Provider=SQLNCLI11.1;Integrated Security=SSPI;</t>
   </si>
   <si>
-    <t>AdventureWorksLT DW</t>
+    <t>StagingTL</t>
+  </si>
+  <si>
+    <t>ProductSales Staging</t>
+  </si>
+  <si>
+    <t>StagingH</t>
+  </si>
+  <si>
+    <t>ProductSales</t>
+  </si>
+  <si>
+    <t>C:\</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>FlatFile</t>
+  </si>
+  <si>
+    <t>.csv</t>
+  </si>
+  <si>
+    <t>Delimited</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>CRLF</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>ItemType</t>
+  </si>
+  <si>
+    <t>FlatFileExtension</t>
+  </si>
+  <si>
+    <t>FlatFileType</t>
+  </si>
+  <si>
+    <t>FlatFileIsUnicode</t>
+  </si>
+  <si>
+    <t>FlatFileColumnDelimiter</t>
+  </si>
+  <si>
+    <t>FlatFileRowDelimiter</t>
+  </si>
+  <si>
+    <t>SSISLoadPattern</t>
+  </si>
+  <si>
+    <t>SSISParallelDataFlows</t>
+  </si>
+  <si>
+    <t>SSISParallelDataFlowsColumn</t>
+  </si>
+  <si>
+    <t>ItemColumnName</t>
+  </si>
+  <si>
+    <t>ScopedItemColumnName</t>
+  </si>
+  <si>
+    <t>Ordinal</t>
+  </si>
+  <si>
+    <t>ChangeType</t>
+  </si>
+  <si>
+    <t>IsNullable</t>
+  </si>
+  <si>
+    <t>IsPrimaryKey</t>
+  </si>
+  <si>
+    <t>IsIdentity</t>
+  </si>
+  <si>
+    <t>DataType</t>
+  </si>
+  <si>
+    <t>DataTypeLength</t>
+  </si>
+  <si>
+    <t>DataTypePrecision</t>
+  </si>
+  <si>
+    <t>DataTypeScale</t>
+  </si>
+  <si>
+    <t>DerivedColumnReplaceExisting</t>
+  </si>
+  <si>
+    <t>DerivedColumnExpression</t>
+  </si>
+  <si>
+    <t>LogicalDisplayFolder</t>
+  </si>
+  <si>
+    <t>ProductNumber</t>
+  </si>
+  <si>
+    <t>Products_ProductNumber</t>
+  </si>
+  <si>
+    <t>AnsiString</t>
+  </si>
+  <si>
+    <t>ProductSales Staging/Products</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Products_ProductName</t>
+  </si>
+  <si>
+    <t>StandardCost</t>
+  </si>
+  <si>
+    <t>Products_StandardCost</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>ListPrice</t>
+  </si>
+  <si>
+    <t>Products_ListPrice</t>
+  </si>
+  <si>
+    <t>SalesID</t>
+  </si>
+  <si>
+    <t>Sales_SalesID</t>
+  </si>
+  <si>
+    <t>Int32</t>
+  </si>
+  <si>
+    <t>ProductSales Staging/Sales</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Sales_FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Sales_LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Sales_Email</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>Sales_Birthdate</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Sales_Gender</t>
+  </si>
+  <si>
+    <t>IPAdress</t>
+  </si>
+  <si>
+    <t>Sales_IPAdress</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>Sales_CountryCode</t>
+  </si>
+  <si>
+    <t>CountryName</t>
+  </si>
+  <si>
+    <t>Sales_CountryName</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>Sales_StateCode</t>
+  </si>
+  <si>
+    <t>StateName</t>
+  </si>
+  <si>
+    <t>Sales_StateName</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Sales_City</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Sales_PostalCode</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Sales_Address</t>
+  </si>
+  <si>
+    <t>CreditCardType</t>
+  </si>
+  <si>
+    <t>Sales_CreditCardType</t>
+  </si>
+  <si>
+    <t>CreditCardNumber</t>
+  </si>
+  <si>
+    <t>Sales_CreditCardNumber</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Sales_Quantity</t>
+  </si>
+  <si>
+    <t>SalesDate</t>
+  </si>
+  <si>
+    <t>Sales_SalesDate</t>
+  </si>
+  <si>
+    <t>Sales_ProductNumber</t>
+  </si>
+  <si>
+    <t>SalesAmount</t>
+  </si>
+  <si>
+    <t>Sales_SalesAmount</t>
+  </si>
+  <si>
+    <t>PSSRC</t>
   </si>
 </sst>
 </file>
@@ -282,6 +554,50 @@
     <tableColumn id="3" name="SourceConnectionName" dataDxfId="2"/>
     <tableColumn id="4" name="DestinationConnectionName" dataDxfId="1"/>
     <tableColumn id="5" name="DestinationSchemaName" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K3" totalsRowShown="0">
+  <autoFilter ref="A1:K3"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="ItemName"/>
+    <tableColumn id="2" name="ItemType"/>
+    <tableColumn id="3" name="ProjectName"/>
+    <tableColumn id="4" name="FlatFileExtension"/>
+    <tableColumn id="5" name="FlatFileType"/>
+    <tableColumn id="6" name="FlatFileIsUnicode"/>
+    <tableColumn id="7" name="FlatFileColumnDelimiter"/>
+    <tableColumn id="8" name="FlatFileRowDelimiter"/>
+    <tableColumn id="9" name="SSISLoadPattern"/>
+    <tableColumn id="10" name="SSISParallelDataFlows"/>
+    <tableColumn id="11" name="SSISParallelDataFlowsColumn"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:O25" totalsRowShown="0">
+  <autoFilter ref="A1:O25"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="ItemName"/>
+    <tableColumn id="2" name="ItemColumnName"/>
+    <tableColumn id="3" name="ScopedItemColumnName"/>
+    <tableColumn id="4" name="Ordinal"/>
+    <tableColumn id="5" name="ChangeType"/>
+    <tableColumn id="6" name="IsNullable"/>
+    <tableColumn id="7" name="IsPrimaryKey"/>
+    <tableColumn id="8" name="IsIdentity"/>
+    <tableColumn id="9" name="DataType"/>
+    <tableColumn id="10" name="DataTypeLength"/>
+    <tableColumn id="11" name="DataTypePrecision"/>
+    <tableColumn id="12" name="DataTypeScale"/>
+    <tableColumn id="13" name="DerivedColumnReplaceExisting"/>
+    <tableColumn id="14" name="DerivedColumnExpression"/>
+    <tableColumn id="15" name="LogicalDisplayFolder"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -895,19 +1211,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -934,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -976,7 +1289,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -996,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -1016,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -1036,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -1056,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
@@ -1073,18 +1386,1293 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.4609375" customWidth="1"/>
+    <col min="2" max="2" width="10.53515625" customWidth="1"/>
+    <col min="3" max="3" width="21.3046875" customWidth="1"/>
+    <col min="4" max="4" width="16.69140625" customWidth="1"/>
+    <col min="5" max="5" width="12.61328125" customWidth="1"/>
+    <col min="6" max="6" width="16.765625" customWidth="1"/>
+    <col min="7" max="7" width="22.61328125" customWidth="1"/>
+    <col min="8" max="8" width="19.921875" customWidth="1"/>
+    <col min="9" max="9" width="16.23046875" customWidth="1"/>
+    <col min="10" max="10" width="20.765625" customWidth="1"/>
+    <col min="11" max="11" width="27.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.07421875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14">
+        <v>50</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>